<commit_message>
Buggfix + update 2023
</commit_message>
<xml_diff>
--- a/indata_valutakurser.xlsx
+++ b/indata_valutakurser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cstrom/Documents/GitHub/k4/SruMaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cstrom/Documents/GitHub/K4SRU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{790A7F17-124F-8442-9FE2-2BBF21182C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BF38B0-5FAB-7A40-95BD-44AFECCE375E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27340" yWindow="8780" windowWidth="27640" windowHeight="16940" xr2:uid="{E3162200-14DF-4F49-A142-99DF38272BEE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{E3162200-14DF-4F49-A142-99DF38272BEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>BRL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CAD</t>
   </si>
@@ -47,12 +41,6 @@
     <t>CHF</t>
   </si>
   <si>
-    <t>CNY</t>
-  </si>
-  <si>
-    <t>CZK</t>
-  </si>
-  <si>
     <t>DKK</t>
   </si>
   <si>
@@ -62,52 +50,7 @@
     <t>GBP</t>
   </si>
   <si>
-    <t>HKD</t>
-  </si>
-  <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>IDR</t>
-  </si>
-  <si>
-    <t>INR</t>
-  </si>
-  <si>
-    <t>ISK</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>KRW</t>
-  </si>
-  <si>
-    <t>MAD</t>
-  </si>
-  <si>
-    <t>MXN</t>
-  </si>
-  <si>
     <t>NOK</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>SAR</t>
-  </si>
-  <si>
-    <t>SGD</t>
-  </si>
-  <si>
-    <t>THB</t>
-  </si>
-  <si>
-    <t>TRY</t>
   </si>
   <si>
     <t>USD</t>
@@ -465,9 +408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD62509E-BDC3-5D41-8A5E-515C0C60F5F1}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -476,26 +421,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1">
-        <v>7.0134999999999996</v>
+        <v>10.6128</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1.9619</v>
+        <v>1.5403</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>7.7712000000000003</v>
+        <v>1.0054000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -503,31 +448,31 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10.59497</v>
+        <v>11.4765</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>1.502</v>
+        <v>7.8636999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>0.43285600000000002</v>
+        <v>11.817299999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>1.4290309999999999</v>
+        <v>13.197900000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -535,159 +480,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>10.6317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>12.466900000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1.2928999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2.7217999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>6.8599999999999998E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0.128666</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>7.4770000000000003E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>7.7074999999999991E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>7.8239999999999994E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0.99609999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>0.50360000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1.052278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>6.4119000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>2.2685</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>2.6962000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>7.3368000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>0.28839999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>0.61350000000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>10.124499999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>0.61819999999999997</v>
+        <v>0.5756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>